<commit_message>
Update Create New Campaign(s).xlsx
</commit_message>
<xml_diff>
--- a/_posts/도서/마케팅/file/Create New Campaign(s).xlsx
+++ b/_posts/도서/마케팅/file/Create New Campaign(s).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\study\shina1221.github.io\_posts\도서\마케팅\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t># Optional.
  Supported values: Add; Edit; Remove.</t>
@@ -65,9 +65,6 @@
     <t>Bid strategy type</t>
   </si>
   <si>
-    <t>Bid strategy</t>
-  </si>
-  <si>
     <t>Campaign start date</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Exclusion</t>
-  </si>
-  <si>
     <t>Devices</t>
   </si>
   <si>
@@ -98,12 +92,6 @@
     <t>Target Impression Share</t>
   </si>
   <si>
-    <t>Max CPC Bid Limit for Target IS</t>
-  </si>
-  <si>
-    <t>Location Goal for Target IS</t>
-  </si>
-  <si>
     <t>Tracking template</t>
   </si>
   <si>
@@ -113,13 +101,7 @@
     <t>Custom parameter</t>
   </si>
   <si>
-    <t>Viewability vendor</t>
-  </si>
-  <si>
     <t>Inventory type</t>
-  </si>
-  <si>
-    <t>Campaign subtype</t>
   </si>
   <si>
     <t>Add</t>
@@ -366,25 +348,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>CPC(enhanced)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>r</t>
-    </r>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>S</t>
     </r>
@@ -399,6 +362,43 @@
     </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>Bid Strategy Name</t>
+  </si>
+  <si>
+    <t>End Date</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Date</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Languages</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exclusion method</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum CPC bid limit</t>
+  </si>
+  <si>
+    <t>Campaign type</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>ko</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enhanced CPC</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ad Location</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +407,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -476,6 +476,13 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="D2Coding"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -503,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -520,6 +527,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -740,8 +750,8 @@
   </sheetPr>
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -769,76 +779,76 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15">
@@ -870,88 +880,84 @@
         <v>12</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="T2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="U2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="AB2" s="7" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G3" s="10">
         <f>5000000/31</f>
         <v>161290.32258064515</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K3" s="11">
         <v>45778</v>
@@ -960,10 +966,10 @@
         <v>45808</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1030,50 +1036,50 @@
         <v>12</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="O1" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4">
         <f>5000000/31</f>
         <v>161290.32258064515</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J2" s="5">
         <v>45778</v>
@@ -1082,16 +1088,16 @@
         <v>45807</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>